<commit_message>
Update Time Series Forecasting - HR.xlsx
</commit_message>
<xml_diff>
--- a/Excel/Time Series Forecasting - HR.xlsx
+++ b/Excel/Time Series Forecasting - HR.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\YT_Time_Series_Forecasting\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D37AEE-1F5E-47A1-9C1A-39C2B9C9379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B152A79-BBDD-4FE1-81B1-82522F395DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{222811F3-B945-4F38-BB77-4DEABE907094}"/>
   </bookViews>
   <sheets>
     <sheet name="Step0" sheetId="4" state="hidden" r:id="rId1"/>
     <sheet name="Step1" sheetId="1" r:id="rId2"/>
-    <sheet name="Step2" sheetId="2" r:id="rId3"/>
-    <sheet name="Step3" sheetId="6" r:id="rId4"/>
-    <sheet name="Step5" sheetId="9" r:id="rId5"/>
-    <sheet name="Step6" sheetId="10" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="13" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId5"/>
+    <sheet name="Step2" sheetId="2" r:id="rId6"/>
+    <sheet name="Step3" sheetId="6" r:id="rId7"/>
+    <sheet name="Step5" sheetId="9" r:id="rId8"/>
+    <sheet name="Step6" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -303,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="99">
   <si>
     <t>Year</t>
   </si>
@@ -505,6 +508,102 @@
   <si>
     <t>Y Pred = 711 + 1466 (time)</t>
   </si>
+  <si>
+    <t>Attrition</t>
+  </si>
+  <si>
+    <t>Hiring</t>
+  </si>
+  <si>
+    <t>MA 3 Active HC</t>
+  </si>
+  <si>
+    <t>Temp MA 4</t>
+  </si>
+  <si>
+    <t>CMA 4 Active HC</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>Forecasted Hiring</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Bus Growth</t>
+  </si>
+  <si>
+    <t>Down Sizing</t>
+  </si>
 </sst>
 </file>
 
@@ -514,9 +613,9 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;?_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;?_ ;_ @_ "/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,6 +693,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -615,7 +722,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -641,6 +748,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -649,7 +804,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -674,7 +829,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -682,6 +837,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -693,6 +851,17 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -756,36 +925,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -831,6 +970,62 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Step1!$B$5:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2015-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2016-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2017-1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2017-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2017-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2018-1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2018-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2018-4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Step1!$E$5:$E$20</c:f>
@@ -892,6 +1087,162 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1A56-4CFA-96DB-25BA2234E447}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Step1!$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MA 3 Active HC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Step1!$B$5:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2015-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2016-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2017-1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2017-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2017-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2018-1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2018-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2018-4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Step1!$F$5:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="1">
+                  <c:v>696.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>753.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>783.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>793.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>846.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>873.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>833.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>836.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>896.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>866.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>873.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>943.33333333333337</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>920</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1A5B-47C9-BB42-F3C371C13974}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -929,6 +1280,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2293,52 +2645,52 @@
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>725</c:v>
+                  <c:v>728.71439482580013</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>739</c:v>
+                  <c:v>743.12181797614176</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>753</c:v>
+                  <c:v>757.52924112648338</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>767</c:v>
+                  <c:v>771.93666427682501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>781</c:v>
+                  <c:v>786.34408742716664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>795</c:v>
+                  <c:v>800.75151057750827</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>809</c:v>
+                  <c:v>815.1589337278499</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>823</c:v>
+                  <c:v>829.56635687819153</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>837</c:v>
+                  <c:v>843.97378002853316</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>851</c:v>
+                  <c:v>858.38120317887478</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>865</c:v>
+                  <c:v>872.78862632921653</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>879</c:v>
+                  <c:v>887.19604947955816</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>893</c:v>
+                  <c:v>901.60347262989978</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>907</c:v>
+                  <c:v>916.01089578024141</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>921</c:v>
+                  <c:v>930.41831893058304</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>935</c:v>
+                  <c:v>944.82574208092467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6644,16 +6996,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>160899</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171669</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>196790</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101967</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>464234</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>13261</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>473998</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>122153</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6678,6 +7030,59 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>816428</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>391614</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DD912F2-CE69-4C16-B167-C5AE0E85F298}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3265714" y="1102179"/>
+          <a:ext cx="1725114" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6686,15 +7091,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>179070</xdr:colOff>
+      <xdr:colOff>347254</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>72864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>437333</xdr:colOff>
+      <xdr:colOff>611232</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>46537</xdr:rowOff>
+      <xdr:rowOff>48442</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7308,27 +7713,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DA07D5-4067-4300-974B-E9B61B517309}">
-  <dimension ref="A2:F24"/>
+  <dimension ref="A2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -7344,8 +7754,25 @@
       <c r="E4" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7358,15 +7785,18 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="30">
         <v>680</v>
       </c>
-      <c r="F5" s="2">
-        <f>E5/100</f>
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J5" s="33"/>
+      <c r="K5" s="2">
+        <v>100</v>
+      </c>
+      <c r="L5" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -7379,15 +7809,23 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="31">
         <v>610</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" ref="F6:F24" si="0">E6/100</f>
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <f>AVERAGE(E5:E7)</f>
+        <v>696.66666666666663</v>
+      </c>
+      <c r="I6" s="16">
+        <f>1-E6/F6</f>
+        <v>0.12440191387559807</v>
+      </c>
+      <c r="K6" s="2">
+        <v>44</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -7400,15 +7838,31 @@
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="31">
         <v>800</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" ref="F7:F20" si="0">AVERAGE(E6:E8)</f>
+        <v>753.33333333333337</v>
+      </c>
+      <c r="G7" s="2">
+        <f>AVERAGE(E5:E8)</f>
+        <v>735</v>
+      </c>
+      <c r="H7" s="2">
+        <f>AVERAGE(G7:G8)</f>
+        <v>747.5</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" ref="I7:I20" si="1">1-E7/F7</f>
+        <v>-6.1946902654867131E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>46</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -7421,15 +7875,31 @@
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="32">
         <v>850</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>810</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G19" si="2">AVERAGE(E6:E9)</f>
+        <v>760</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:H18" si="3">AVERAGE(G8:G9)</f>
+        <v>773.75</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="1"/>
+        <v>-4.9382716049382713E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>56</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -7447,10 +7917,26 @@
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>783.33333333333337</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>787.5</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="3"/>
+        <v>797.5</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="1"/>
+        <v>4.2553191489361764E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>59</v>
+      </c>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -7468,10 +7954,26 @@
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>793.33333333333337</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>807.5</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="3"/>
+        <v>818.75</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="1"/>
+        <v>9.2436974789915971E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>45</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -7489,10 +7991,26 @@
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>846.66666666666663</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>830</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="3"/>
+        <v>832.5</v>
+      </c>
+      <c r="I11" s="16">
+        <f t="shared" si="1"/>
+        <v>-3.9370078740157632E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>36</v>
+      </c>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -7510,10 +8028,26 @@
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>873.33333333333337</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>835</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="3"/>
+        <v>840</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="1"/>
+        <v>-7.6335877862595325E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>55</v>
+      </c>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -7531,10 +8065,26 @@
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>833.33333333333337</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="2"/>
+        <v>845</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="3"/>
+        <v>853.75</v>
+      </c>
+      <c r="I13" s="16">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="K13" s="2">
+        <v>30</v>
+      </c>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -7552,10 +8102,26 @@
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>836.66666666666663</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>862.5</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="3"/>
+        <v>867.5</v>
+      </c>
+      <c r="I14" s="16">
+        <f t="shared" si="1"/>
+        <v>9.1633466135458086E-2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>33</v>
+      </c>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -7573,10 +8139,26 @@
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>896.66666666666663</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="2"/>
+        <v>872.5</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="3"/>
+        <v>876.25</v>
+      </c>
+      <c r="I15" s="16">
+        <f t="shared" si="1"/>
+        <v>-5.9479553903345694E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>59</v>
+      </c>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -7594,10 +8176,26 @@
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>9.8000000000000007</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="2"/>
+        <v>880</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="3"/>
+        <v>883.75</v>
+      </c>
+      <c r="I16" s="16">
+        <f t="shared" si="1"/>
+        <v>-6.5217391304347894E-2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>38</v>
+      </c>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -7615,10 +8213,26 @@
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>866.66666666666663</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="2"/>
+        <v>887.5</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="3"/>
+        <v>893.75</v>
+      </c>
+      <c r="I17" s="16">
+        <f t="shared" si="1"/>
+        <v>4.2307692307692268E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <v>40</v>
+      </c>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -7636,10 +8250,26 @@
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>873.33333333333337</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="2"/>
+        <v>900</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="3"/>
+        <v>907.5</v>
+      </c>
+      <c r="I18" s="16">
+        <f t="shared" si="1"/>
+        <v>9.5419847328244267E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>55</v>
+      </c>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -7657,10 +8287,22 @@
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>943.33333333333337</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="2"/>
+        <v>915</v>
+      </c>
+      <c r="I19" s="16">
+        <f t="shared" si="1"/>
+        <v>-6.0070671378091856E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>46</v>
+      </c>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -7677,37 +8319,96 @@
         <v>1040</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>10.4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <f>F16</f>
+        <v>920</v>
+      </c>
+      <c r="I20" s="16">
+        <f>I16</f>
+        <v>-6.5217391304347894E-2</v>
+      </c>
+      <c r="K20" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="18">
+        <f>F21+(F21*I21)</f>
+        <v>903.33333333333326</v>
+      </c>
+      <c r="F21" s="2">
+        <f>F17</f>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="I21" s="33">
+        <f>I17</f>
+        <v>4.2307692307692268E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="18">
+        <f t="shared" ref="E22:E24" si="4">F22+(F22*I22)</f>
+        <v>956.66666666666674</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" ref="F22:F24" si="5">F18</f>
+        <v>873.33333333333337</v>
+      </c>
+      <c r="I22" s="33">
+        <f t="shared" ref="I22:I24" si="6">I18</f>
+        <v>9.5419847328244267E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" s="18">
+        <f t="shared" si="4"/>
+        <v>886.66666666666674</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="5"/>
+        <v>943.33333333333337</v>
+      </c>
+      <c r="I23" s="33">
+        <f t="shared" si="6"/>
+        <v>-6.0070671378091856E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="2"/>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" s="18">
+        <f t="shared" si="4"/>
+        <v>859.99999999999989</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="5"/>
+        <v>920</v>
+      </c>
+      <c r="I24" s="33">
+        <f t="shared" si="6"/>
+        <v>-6.5217391304347894E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7719,11 +8420,817 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B2D389-F389-4014-8E07-870692447BED}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="35"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.43995905444776329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.19356396959056993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="9">
+        <v>6.9496887989119155E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="9">
+        <v>116.19471780441603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>42127.988206577604</v>
+      </c>
+      <c r="D12" s="9">
+        <v>21063.994103288802</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1.5601557406852593</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.2470042925837613</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="9">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9">
+        <v>175515.7617934224</v>
+      </c>
+      <c r="D13" s="9">
+        <v>13501.212445647876</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="10">
+        <v>15</v>
+      </c>
+      <c r="C14" s="10">
+        <v>217643.75</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="9">
+        <v>875.8790493997642</v>
+      </c>
+      <c r="C17" s="9">
+        <v>64.097588939767803</v>
+      </c>
+      <c r="D17" s="9">
+        <v>13.664773728428749</v>
+      </c>
+      <c r="E17" s="9">
+        <v>4.3356073853473388E-9</v>
+      </c>
+      <c r="F17" s="9">
+        <v>737.40462729945364</v>
+      </c>
+      <c r="G17" s="9">
+        <v>1014.3534715000748</v>
+      </c>
+      <c r="H17" s="9">
+        <v>737.40462729945364</v>
+      </c>
+      <c r="I17" s="9">
+        <v>1014.3534715000748</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.19067470286389526</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.59265749637667287</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.32172832374452737</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.75277311408438019</v>
+      </c>
+      <c r="F18" s="9">
+        <v>-1.0896839763259798</v>
+      </c>
+      <c r="G18" s="9">
+        <v>1.4710333820537704</v>
+      </c>
+      <c r="H18" s="9">
+        <v>-1.0896839763259798</v>
+      </c>
+      <c r="I18" s="9">
+        <v>1.4710333820537704</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="10">
+        <v>-0.54874451918049538</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.34522333699052743</v>
+      </c>
+      <c r="D19" s="10">
+        <v>-1.5895348326221421</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.13595431839827468</v>
+      </c>
+      <c r="F19" s="10">
+        <v>-1.2945541958943232</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.19706515753333231</v>
+      </c>
+      <c r="H19" s="10">
+        <v>-1.2945541958943232</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.19706515753333231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB08370-292B-42EC-8C11-DBD885B562EF}">
+  <dimension ref="B2:L19"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="9">
+        <v>875.8790493997642</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>680</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="G4" s="36">
+        <f>$L$3+$L$4*C4+$L$5*D4</f>
+        <v>878.48418411073885</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.19067470286389526</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>610</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>234</v>
+      </c>
+      <c r="G5" s="36">
+        <f>$L$3+$L$4*C5+$L$5*D5</f>
+        <v>755.8625188375396</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="10">
+        <v>-0.54874451918049538</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>800</v>
+      </c>
+      <c r="C6">
+        <v>46</v>
+      </c>
+      <c r="D6">
+        <v>96</v>
+      </c>
+      <c r="G6" s="36">
+        <f>$L$3+$L$4*C6+$L$5*D6</f>
+        <v>831.97061189017586</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>850</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="36">
+        <f>$L$3+$L$4*C7+$L$5*D7</f>
+        <v>887.43592951865389</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>780</v>
+      </c>
+      <c r="C8">
+        <v>65</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="G8" s="36">
+        <f>$L$3+$L$4*C8+$L$5*D8</f>
+        <v>885.52918249001493</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>720</v>
+      </c>
+      <c r="C9">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>205</v>
+      </c>
+      <c r="G9" s="36">
+        <f>$L$3+$L$4*C9+$L$5*D9</f>
+        <v>771.96678459663792</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>880</v>
+      </c>
+      <c r="C10">
+        <v>36</v>
+      </c>
+      <c r="D10">
+        <v>96</v>
+      </c>
+      <c r="G10" s="36">
+        <f>$L$3+$L$4*C10+$L$5*D10</f>
+        <v>830.0638648615369</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>940</v>
+      </c>
+      <c r="C11">
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="G11" s="36">
+        <f>$L$3+$L$4*C11+$L$5*D11</f>
+        <v>881.08931882171362</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>800</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="36">
+        <f>$L$3+$L$4*C12+$L$5*D12</f>
+        <v>879.92533935115409</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>760</v>
+      </c>
+      <c r="C13">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>223</v>
+      </c>
+      <c r="G13" s="36">
+        <f>$L$3+$L$4*C13+$L$5*D13</f>
+        <v>759.80128681702229</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>950</v>
+      </c>
+      <c r="C14">
+        <v>59</v>
+      </c>
+      <c r="D14">
+        <v>89</v>
+      </c>
+      <c r="G14" s="36">
+        <f>$L$3+$L$4*C14+$L$5*D14</f>
+        <v>838.29059466166996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>980</v>
+      </c>
+      <c r="C15">
+        <v>180</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="G15" s="36">
+        <f>$L$3+$L$4*C15+$L$5*D15</f>
+        <v>893.73816033985054</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>830</v>
+      </c>
+      <c r="C16">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="36">
+        <f>$L$3+$L$4*C16+$L$5*D16</f>
+        <v>883.50603751432004</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>790</v>
+      </c>
+      <c r="C17">
+        <v>55</v>
+      </c>
+      <c r="D17">
+        <v>265</v>
+      </c>
+      <c r="G17" s="36">
+        <f>$L$3+$L$4*C17+$L$5*D17</f>
+        <v>740.9488604744472</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>1000</v>
+      </c>
+      <c r="C18">
+        <v>46</v>
+      </c>
+      <c r="D18">
+        <v>86</v>
+      </c>
+      <c r="G18" s="36">
+        <f>$L$3+$L$4*C18+$L$5*D18</f>
+        <v>837.45805708198077</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>1040</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+      <c r="G19" s="36">
+        <f>$L$3+$L$4*C19+$L$5*D19</f>
+        <v>853.92926863254434</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E31D6AB-9BD6-4742-ABF8-D33DFAECA0AC}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="35"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.95429581729512514</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.91068050690697089</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.90380977666904561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="9">
+        <v>20.940341297487453</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>58120.675713240067</v>
+      </c>
+      <c r="D12" s="9">
+        <v>58120.675713240067</v>
+      </c>
+      <c r="E12" s="9">
+        <v>132.54493705489452</v>
+      </c>
+      <c r="F12" s="9">
+        <v>3.42997973865757E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="9">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9">
+        <v>5700.4726175183596</v>
+      </c>
+      <c r="D13" s="9">
+        <v>438.49789365525845</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="10">
+        <v>14</v>
+      </c>
+      <c r="C14" s="10">
+        <v>63821.148330758428</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="9">
+        <v>714.3069716754585</v>
+      </c>
+      <c r="C17" s="9">
+        <v>12.493373014890462</v>
+      </c>
+      <c r="D17" s="9">
+        <v>57.174869494739191</v>
+      </c>
+      <c r="E17" s="9">
+        <v>5.2860595594683017E-17</v>
+      </c>
+      <c r="F17" s="9">
+        <v>687.31668020059112</v>
+      </c>
+      <c r="G17" s="9">
+        <v>741.29726315032588</v>
+      </c>
+      <c r="H17" s="9">
+        <v>687.31668020059112</v>
+      </c>
+      <c r="I17" s="9">
+        <v>741.29726315032588</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10">
+        <v>14.407423150341636</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1.2514247503991749</v>
+      </c>
+      <c r="D18" s="10">
+        <v>11.512816208682151</v>
+      </c>
+      <c r="E18" s="10">
+        <v>3.4299797386575819E-8</v>
+      </c>
+      <c r="F18" s="10">
+        <v>11.703884343657485</v>
+      </c>
+      <c r="G18" s="10">
+        <v>17.110961957025786</v>
+      </c>
+      <c r="H18" s="10">
+        <v>11.703884343657485</v>
+      </c>
+      <c r="I18" s="10">
+        <v>17.110961957025786</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DA9F5E-4978-4CC8-9AB3-607969F7620D}">
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7768,13 +9275,13 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
       <c r="N5">
         <v>4</v>
       </c>
@@ -7787,10 +9294,10 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="28"/>
       <c r="H6" t="s">
         <v>10</v>
       </c>
@@ -8397,12 +9904,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4F9F03-510D-453C-A3C8-DE8A0089C8A2}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E24"/>
+      <selection activeCell="K28" sqref="K28:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8424,8 +9931,8 @@
       <c r="Q1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="11">
-        <v>711</v>
+      <c r="R1" s="9">
+        <v>714.3069716754585</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8439,8 +9946,8 @@
       <c r="Q2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="12">
-        <v>14</v>
+      <c r="R2" s="10">
+        <v>14.407423150341636</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -8493,10 +10000,10 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="28"/>
       <c r="H7" t="s">
         <v>10</v>
       </c>
@@ -8568,7 +10075,7 @@
       </c>
       <c r="K9" s="2">
         <f>$R$1+A9*$R$2</f>
-        <v>725</v>
+        <v>728.71439482580013</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -8596,8 +10103,8 @@
         <v>696.87912606554323</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" ref="K10:K28" si="2">$R$1+A10*$R$2</f>
-        <v>739</v>
+        <f t="shared" ref="K10:K32" si="2">$R$1+A10*$R$2</f>
+        <v>743.12181797614176</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -8638,7 +10145,7 @@
       </c>
       <c r="K11" s="2">
         <f t="shared" si="2"/>
-        <v>753</v>
+        <v>757.52924112648338</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -8679,7 +10186,7 @@
       </c>
       <c r="K12" s="2">
         <f t="shared" si="2"/>
-        <v>767</v>
+        <v>771.93666427682501</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -8720,7 +10227,7 @@
       </c>
       <c r="K13" s="2">
         <f t="shared" si="2"/>
-        <v>781</v>
+        <v>786.34408742716664</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -8761,7 +10268,7 @@
       </c>
       <c r="K14" s="2">
         <f t="shared" si="2"/>
-        <v>795</v>
+        <v>800.75151057750827</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -8802,7 +10309,7 @@
       </c>
       <c r="K15" s="2">
         <f t="shared" si="2"/>
-        <v>809</v>
+        <v>815.1589337278499</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -8843,7 +10350,7 @@
       </c>
       <c r="K16" s="2">
         <f t="shared" si="2"/>
-        <v>823</v>
+        <v>829.56635687819153</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -8884,7 +10391,7 @@
       </c>
       <c r="K17" s="2">
         <f t="shared" si="2"/>
-        <v>837</v>
+        <v>843.97378002853316</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -8925,7 +10432,7 @@
       </c>
       <c r="K18" s="2">
         <f t="shared" si="2"/>
-        <v>851</v>
+        <v>858.38120317887478</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -8966,7 +10473,7 @@
       </c>
       <c r="K19" s="2">
         <f t="shared" si="2"/>
-        <v>865</v>
+        <v>872.78862632921653</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -9007,7 +10514,7 @@
       </c>
       <c r="K20" s="2">
         <f t="shared" si="2"/>
-        <v>879</v>
+        <v>887.19604947955816</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -9048,7 +10555,7 @@
       </c>
       <c r="K21" s="2">
         <f t="shared" si="2"/>
-        <v>893</v>
+        <v>901.60347262989978</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -9089,7 +10596,7 @@
       </c>
       <c r="K22" s="2">
         <f t="shared" si="2"/>
-        <v>907</v>
+        <v>916.01089578024141</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -9123,7 +10630,7 @@
       </c>
       <c r="K23" s="2">
         <f t="shared" si="2"/>
-        <v>921</v>
+        <v>930.41831893058304</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -9153,7 +10660,7 @@
       </c>
       <c r="K24" s="2">
         <f t="shared" si="2"/>
-        <v>935</v>
+        <v>944.82574208092467</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -9175,7 +10682,7 @@
       </c>
       <c r="K25" s="22">
         <f t="shared" si="2"/>
-        <v>949</v>
+        <v>959.2331652312663</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -9196,8 +10703,8 @@
         <v>0.8753311401992373</v>
       </c>
       <c r="K26" s="22">
-        <f t="shared" si="2"/>
-        <v>963</v>
+        <f>$R$1+A26*$R$2</f>
+        <v>973.64058838160793</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -9219,7 +10726,7 @@
       </c>
       <c r="K27" s="22">
         <f t="shared" si="2"/>
-        <v>977</v>
+        <v>988.04801153194956</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -9241,7 +10748,43 @@
       </c>
       <c r="K28" s="22">
         <f t="shared" si="2"/>
-        <v>991</v>
+        <v>1002.4554346822912</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="20">
+        <v>21</v>
+      </c>
+      <c r="K29" s="22">
+        <f t="shared" si="2"/>
+        <v>1016.8628578326329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="20">
+        <v>22</v>
+      </c>
+      <c r="K30" s="22">
+        <f t="shared" si="2"/>
+        <v>1031.2702809829746</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="20">
+        <v>23</v>
+      </c>
+      <c r="K31" s="22">
+        <f t="shared" si="2"/>
+        <v>1045.6777041333162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="20">
+        <v>24</v>
+      </c>
+      <c r="K32" s="22">
+        <f t="shared" si="2"/>
+        <v>1060.0851272836578</v>
       </c>
     </row>
   </sheetData>
@@ -9254,12 +10797,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D3E6A3-3885-4160-8830-D576A1D5B683}">
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9343,7 +10886,7 @@
       <c r="J6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="29" t="s">
         <v>63</v>
       </c>
     </row>
@@ -9351,17 +10894,17 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="28"/>
       <c r="H7" t="s">
         <v>10</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="28"/>
+      <c r="L7" s="29"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
@@ -10194,7 +11737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7077317-5789-49E2-9FD1-ACE8A18EC299}">
   <dimension ref="A1:T28"/>
   <sheetViews>
@@ -10305,21 +11848,21 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="28"/>
       <c r="H7" t="s">
         <v>10</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>